<commit_message>
cleaning of commune data
</commit_message>
<xml_diff>
--- a/data/statistik-steuerfuesse-np-1995-2023-fr.xlsx
+++ b/data/statistik-steuerfuesse-np-1995-2023-fr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/A HEC/Master/Semestre 2/Machine Learning/Machine_Learning/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2311D9-9C61-E14C-853D-00DF330146A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC07302-91E6-3F42-8833-BD34665A2953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6360" yWindow="500" windowWidth="21000" windowHeight="17500" tabRatio="923" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4239,8 +4239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71261DFA-A9E4-41D9-876B-E5EAA66F299C}">
   <dimension ref="B2:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>